<commit_message>
Buff-Mult - BOM temp spreadsheet
</commit_message>
<xml_diff>
--- a/modules/Buff-Mult/Buff-Mult-BOM.xlsx
+++ b/modules/Buff-Mult/Buff-Mult-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Buff-Mult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9AF654B1-543A-4D47-B3F6-C7D719191A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3E9FA5-8FA9-4801-B711-C630B94128EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1485" windowWidth="19665" windowHeight="11385"/>
+    <workbookView xWindow="5280" yWindow="1485" windowWidth="19665" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buff-Mult-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -406,7 +418,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1252,11 +1264,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,9 +1348,12 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <f>MAX(B2-(C2+D2),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1375,9 +1390,12 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="0">B3-(C3+D3)</f>
-        <v>2</v>
+        <f t="shared" ref="E3:E13" si="0">MAX(B3-(C3+D3),0)</f>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -1426,9 +1444,12 @@
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
@@ -1465,9 +1486,12 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
@@ -1501,9 +1525,12 @@
       <c r="B6">
         <v>8</v>
       </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>59</v>
@@ -1555,9 +1582,12 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>71</v>
@@ -1594,9 +1624,12 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>78</v>
@@ -1633,9 +1666,12 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>84</v>
@@ -1678,9 +1714,12 @@
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>93</v>
@@ -1717,9 +1756,12 @@
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>102</v>
@@ -1756,9 +1798,12 @@
       <c r="B12">
         <v>6</v>
       </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>110</v>
@@ -1798,9 +1843,12 @@
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
Buff-Mult - BOM update
</commit_message>
<xml_diff>
--- a/modules/Buff-Mult/Buff-Mult-BOM.xlsx
+++ b/modules/Buff-Mult/Buff-Mult-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Buff-Mult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3E9FA5-8FA9-4801-B711-C630B94128EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BFA8DF-286D-46B3-A31D-04A10227FA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1485" windowWidth="19665" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="2040" windowWidth="19110" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buff-Mult-BOM" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,9 +1801,12 @@
       <c r="C12">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>110</v>

</xml_diff>